<commit_message>
printing, buffer back, color
</commit_message>
<xml_diff>
--- a/docs/fullDFA.xlsx
+++ b/docs/fullDFA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karlm\Desktop\activegits\Compiler\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6ABF6837-3985-4FFE-8D81-A613BC98B220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A281EB2-190F-42E9-97AF-FCFB123BECCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2775" yWindow="840" windowWidth="19455" windowHeight="15075" xr2:uid="{793E41E3-A8D2-4B81-8F44-A7735E5B5AB8}"/>
+    <workbookView xWindow="3240" yWindow="390" windowWidth="19455" windowHeight="15075" xr2:uid="{793E41E3-A8D2-4B81-8F44-A7735E5B5AB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1941" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="210">
   <si>
     <t>B</t>
   </si>
@@ -667,6 +667,9 @@
   <si>
     <t>STATE_FALSE, FALSEOP, 1</t>
   </si>
+  <si>
+    <t>STATE_MINUS, INTLITERAL, 1</t>
+  </si>
 </sst>
 </file>
 
@@ -1020,10 +1023,10 @@
   <dimension ref="A1:AX80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R22" sqref="R22"/>
+      <selection pane="bottomRight" activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,107 +1192,107 @@
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="C3" t="str">
-        <f>_xlfn.CONCAT("CH_",C1)</f>
+        <f t="shared" ref="C3:AB3" si="1">_xlfn.CONCAT("CH_",C1)</f>
         <v>CH_A</v>
       </c>
       <c r="D3" t="str">
-        <f>_xlfn.CONCAT("CH_",D1)</f>
+        <f t="shared" si="1"/>
         <v>CH_B</v>
       </c>
       <c r="E3" t="str">
-        <f>_xlfn.CONCAT("CH_",E1)</f>
+        <f t="shared" si="1"/>
         <v>CH_C</v>
       </c>
       <c r="F3" t="str">
-        <f>_xlfn.CONCAT("CH_",F1)</f>
+        <f t="shared" si="1"/>
         <v>CH_D</v>
       </c>
       <c r="G3" t="str">
-        <f>_xlfn.CONCAT("CH_",G1)</f>
+        <f t="shared" si="1"/>
         <v>CH_E</v>
       </c>
       <c r="H3" t="str">
-        <f>_xlfn.CONCAT("CH_",H1)</f>
+        <f t="shared" si="1"/>
         <v>CH_F</v>
       </c>
       <c r="I3" t="str">
-        <f>_xlfn.CONCAT("CH_",I1)</f>
+        <f t="shared" si="1"/>
         <v>CH_G</v>
       </c>
       <c r="J3" t="str">
-        <f>_xlfn.CONCAT("CH_",J1)</f>
+        <f t="shared" si="1"/>
         <v>CH_H</v>
       </c>
       <c r="K3" t="str">
-        <f>_xlfn.CONCAT("CH_",K1)</f>
+        <f t="shared" si="1"/>
         <v>CH_I</v>
       </c>
       <c r="L3" t="str">
-        <f>_xlfn.CONCAT("CH_",L1)</f>
+        <f t="shared" si="1"/>
         <v>CH_J</v>
       </c>
       <c r="M3" t="str">
-        <f>_xlfn.CONCAT("CH_",M1)</f>
+        <f t="shared" si="1"/>
         <v>CH_K</v>
       </c>
       <c r="N3" t="str">
-        <f>_xlfn.CONCAT("CH_",N1)</f>
+        <f t="shared" si="1"/>
         <v>CH_L</v>
       </c>
       <c r="O3" t="str">
-        <f>_xlfn.CONCAT("CH_",O1)</f>
+        <f t="shared" si="1"/>
         <v>CH_M</v>
       </c>
       <c r="P3" t="str">
-        <f>_xlfn.CONCAT("CH_",P1)</f>
+        <f t="shared" si="1"/>
         <v>CH_N</v>
       </c>
       <c r="Q3" t="str">
-        <f>_xlfn.CONCAT("CH_",Q1)</f>
+        <f t="shared" si="1"/>
         <v>CH_O</v>
       </c>
       <c r="R3" t="str">
-        <f>_xlfn.CONCAT("CH_",R1)</f>
+        <f t="shared" si="1"/>
         <v>CH_P</v>
       </c>
       <c r="S3" t="str">
-        <f>_xlfn.CONCAT("CH_",S1)</f>
+        <f t="shared" si="1"/>
         <v>CH_Q</v>
       </c>
       <c r="T3" t="str">
-        <f>_xlfn.CONCAT("CH_",T1)</f>
+        <f t="shared" si="1"/>
         <v>CH_R</v>
       </c>
       <c r="U3" t="str">
-        <f>_xlfn.CONCAT("CH_",U1)</f>
+        <f t="shared" si="1"/>
         <v>CH_S</v>
       </c>
       <c r="V3" t="str">
-        <f>_xlfn.CONCAT("CH_",V1)</f>
+        <f t="shared" si="1"/>
         <v>CH_T</v>
       </c>
       <c r="W3" t="str">
-        <f>_xlfn.CONCAT("CH_",W1)</f>
+        <f t="shared" si="1"/>
         <v>CH_U</v>
       </c>
       <c r="X3" t="str">
-        <f>_xlfn.CONCAT("CH_",X1)</f>
+        <f t="shared" si="1"/>
         <v>CH_V</v>
       </c>
       <c r="Y3" t="str">
-        <f>_xlfn.CONCAT("CH_",Y1)</f>
+        <f t="shared" si="1"/>
         <v>CH_W</v>
       </c>
       <c r="Z3" t="str">
-        <f>_xlfn.CONCAT("CH_",Z1)</f>
+        <f t="shared" si="1"/>
         <v>CH_X</v>
       </c>
       <c r="AA3" t="str">
-        <f>_xlfn.CONCAT("CH_",AA1)</f>
+        <f t="shared" si="1"/>
         <v>CH_Y</v>
       </c>
       <c r="AB3" t="str">
-        <f>_xlfn.CONCAT("CH_",AB1)</f>
+        <f t="shared" si="1"/>
         <v>CH_Z</v>
       </c>
       <c r="AC3" t="s">
@@ -1364,177 +1367,177 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:AT4" si="1">D4+1</f>
+        <f t="shared" ref="E4:AT4" si="2">D4+1</f>
         <v>2</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="J4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="K4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="L4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="M4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="N4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="O4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="P4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="R4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="S4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="T4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="U4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="V4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="W4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="X4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="Z4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="AA4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="AB4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="AC4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="AD4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="AE4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="AF4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="AG4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="AH4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="AI4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="AJ4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="AK4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="AL4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="AM4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="AN4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="AO4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="AP4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="AQ4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="AR4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="AS4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="AT4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f>_xlfn.CONCAT("STATE_",B5)</f>
+        <f t="shared" ref="A5:A36" si="3">_xlfn.CONCAT("STATE_",B5)</f>
         <v>STATE_START</v>
       </c>
       <c r="B5" t="s">
@@ -1621,7 +1624,7 @@
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f>_xlfn.CONCAT("STATE_",B6)</f>
+        <f t="shared" si="3"/>
         <v>STATE_ID</v>
       </c>
       <c r="B6" t="s">
@@ -1684,7 +1687,7 @@
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f>_xlfn.CONCAT("STATE_",B7)</f>
+        <f t="shared" si="3"/>
         <v>STATE_ERROR</v>
       </c>
       <c r="B7" t="s">
@@ -1825,7 +1828,7 @@
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f>_xlfn.CONCAT("STATE_",B8)</f>
+        <f t="shared" si="3"/>
         <v>STATE_B</v>
       </c>
       <c r="B8" t="s">
@@ -1891,7 +1894,7 @@
     </row>
     <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f>_xlfn.CONCAT("STATE_",B9)</f>
+        <f t="shared" si="3"/>
         <v>STATE_BE</v>
       </c>
       <c r="B9" t="s">
@@ -1957,7 +1960,7 @@
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f>_xlfn.CONCAT("STATE_",B10)</f>
+        <f t="shared" si="3"/>
         <v>STATE_BEG</v>
       </c>
       <c r="B10" t="s">
@@ -2023,7 +2026,7 @@
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>_xlfn.CONCAT("STATE_",B11)</f>
+        <f t="shared" si="3"/>
         <v>STATE_BEGI</v>
       </c>
       <c r="B11" t="s">
@@ -2089,7 +2092,7 @@
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>_xlfn.CONCAT("STATE_",B12)</f>
+        <f t="shared" si="3"/>
         <v>STATE_BEGIN</v>
       </c>
       <c r="B12" t="s">
@@ -2152,7 +2155,7 @@
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>_xlfn.CONCAT("STATE_",B13)</f>
+        <f t="shared" si="3"/>
         <v>STATE_E</v>
       </c>
       <c r="B13" t="s">
@@ -2221,7 +2224,7 @@
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f>_xlfn.CONCAT("STATE_",B14)</f>
+        <f t="shared" si="3"/>
         <v>STATE_EN</v>
       </c>
       <c r="B14" t="s">
@@ -2287,7 +2290,7 @@
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f>_xlfn.CONCAT("STATE_",B15)</f>
+        <f t="shared" si="3"/>
         <v>STATE_END</v>
       </c>
       <c r="B15" t="s">
@@ -2356,7 +2359,7 @@
     </row>
     <row r="16" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f>_xlfn.CONCAT("STATE_",B16)</f>
+        <f t="shared" si="3"/>
         <v>STATE_R</v>
       </c>
       <c r="B16" t="s">
@@ -2422,7 +2425,7 @@
     </row>
     <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f>_xlfn.CONCAT("STATE_",B17)</f>
+        <f t="shared" si="3"/>
         <v>STATE_RE</v>
       </c>
       <c r="B17" t="s">
@@ -2488,7 +2491,7 @@
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f>_xlfn.CONCAT("STATE_",B18)</f>
+        <f t="shared" si="3"/>
         <v>STATE_REA</v>
       </c>
       <c r="B18" t="s">
@@ -2554,7 +2557,7 @@
     </row>
     <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f>_xlfn.CONCAT("STATE_",B19)</f>
+        <f t="shared" si="3"/>
         <v>STATE_READ</v>
       </c>
       <c r="B19" t="s">
@@ -2617,7 +2620,7 @@
     </row>
     <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f>_xlfn.CONCAT("STATE_",B20)</f>
+        <f t="shared" si="3"/>
         <v>STATE_I</v>
       </c>
       <c r="B20" t="s">
@@ -2683,7 +2686,7 @@
     </row>
     <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f>_xlfn.CONCAT("STATE_",B21)</f>
+        <f t="shared" si="3"/>
         <v>STATE_IF</v>
       </c>
       <c r="B21" t="s">
@@ -2746,7 +2749,7 @@
     </row>
     <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f>_xlfn.CONCAT("STATE_",B22)</f>
+        <f t="shared" si="3"/>
         <v>STATE_T</v>
       </c>
       <c r="B22" t="s">
@@ -2815,7 +2818,7 @@
     </row>
     <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f>_xlfn.CONCAT("STATE_",B23)</f>
+        <f t="shared" si="3"/>
         <v>STATE_TH</v>
       </c>
       <c r="B23" t="s">
@@ -2881,7 +2884,7 @@
     </row>
     <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f>_xlfn.CONCAT("STATE_",B24)</f>
+        <f t="shared" si="3"/>
         <v>STATE_THE</v>
       </c>
       <c r="B24" t="s">
@@ -2947,7 +2950,7 @@
     </row>
     <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>_xlfn.CONCAT("STATE_",B25)</f>
+        <f t="shared" si="3"/>
         <v>STATE_THEN</v>
       </c>
       <c r="B25" t="s">
@@ -3010,7 +3013,7 @@
     </row>
     <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f>_xlfn.CONCAT("STATE_",B26)</f>
+        <f t="shared" si="3"/>
         <v>STATE_EL</v>
       </c>
       <c r="B26" t="s">
@@ -3076,7 +3079,7 @@
     </row>
     <row r="27" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f>_xlfn.CONCAT("STATE_",B27)</f>
+        <f t="shared" si="3"/>
         <v>STATE_ELS</v>
       </c>
       <c r="B27" t="s">
@@ -3142,7 +3145,7 @@
     </row>
     <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f>_xlfn.CONCAT("STATE_",B28)</f>
+        <f t="shared" si="3"/>
         <v>STATE_ELSE</v>
       </c>
       <c r="B28" t="s">
@@ -3205,7 +3208,7 @@
     </row>
     <row r="29" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f>_xlfn.CONCAT("STATE_",B29)</f>
+        <f t="shared" si="3"/>
         <v>STATE_ENDI</v>
       </c>
       <c r="B29" t="s">
@@ -3271,7 +3274,7 @@
     </row>
     <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
-        <f>_xlfn.CONCAT("STATE_",B30)</f>
+        <f t="shared" si="3"/>
         <v>STATE_ENDIF</v>
       </c>
       <c r="B30" t="s">
@@ -3334,7 +3337,7 @@
     </row>
     <row r="31" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f>_xlfn.CONCAT("STATE_",B31)</f>
+        <f t="shared" si="3"/>
         <v>STATE_ENDW</v>
       </c>
       <c r="B31" t="s">
@@ -3400,7 +3403,7 @@
     </row>
     <row r="32" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f>_xlfn.CONCAT("STATE_",B32)</f>
+        <f t="shared" si="3"/>
         <v>STATE_ENDWH</v>
       </c>
       <c r="B32" t="s">
@@ -3466,7 +3469,7 @@
     </row>
     <row r="33" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f>_xlfn.CONCAT("STATE_",B33)</f>
+        <f t="shared" si="3"/>
         <v>STATE_ENDWHI</v>
       </c>
       <c r="B33" t="s">
@@ -3532,7 +3535,7 @@
     </row>
     <row r="34" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f>_xlfn.CONCAT("STATE_",B34)</f>
+        <f t="shared" si="3"/>
         <v>STATE_ENDWHIL</v>
       </c>
       <c r="B34" t="s">
@@ -3598,7 +3601,7 @@
     </row>
     <row r="35" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f>_xlfn.CONCAT("STATE_",B35)</f>
+        <f t="shared" si="3"/>
         <v>STATE_ENDWHILE</v>
       </c>
       <c r="B35" t="s">
@@ -3661,7 +3664,7 @@
     </row>
     <row r="36" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f>_xlfn.CONCAT("STATE_",B36)</f>
+        <f t="shared" si="3"/>
         <v>STATE_W</v>
       </c>
       <c r="B36" t="s">
@@ -3730,7 +3733,7 @@
     </row>
     <row r="37" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f>_xlfn.CONCAT("STATE_",B37)</f>
+        <f t="shared" ref="A37:A68" si="4">_xlfn.CONCAT("STATE_",B37)</f>
         <v>STATE_WH</v>
       </c>
       <c r="B37" t="s">
@@ -3796,7 +3799,7 @@
     </row>
     <row r="38" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f>_xlfn.CONCAT("STATE_",B38)</f>
+        <f t="shared" si="4"/>
         <v>STATE_WHI</v>
       </c>
       <c r="B38" t="s">
@@ -3862,7 +3865,7 @@
     </row>
     <row r="39" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f>_xlfn.CONCAT("STATE_",B39)</f>
+        <f t="shared" si="4"/>
         <v>STATE_WHIL</v>
       </c>
       <c r="B39" t="s">
@@ -3928,7 +3931,7 @@
     </row>
     <row r="40" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f>_xlfn.CONCAT("STATE_",B40)</f>
+        <f t="shared" si="4"/>
         <v>STATE_WHILE</v>
       </c>
       <c r="B40" t="s">
@@ -3991,7 +3994,7 @@
     </row>
     <row r="41" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f>_xlfn.CONCAT("STATE_",B41)</f>
+        <f t="shared" si="4"/>
         <v>STATE_F</v>
       </c>
       <c r="B41" t="s">
@@ -4057,7 +4060,7 @@
     </row>
     <row r="42" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f>_xlfn.CONCAT("STATE_",B42)</f>
+        <f t="shared" si="4"/>
         <v>STATE_FA</v>
       </c>
       <c r="B42" t="s">
@@ -4123,7 +4126,7 @@
     </row>
     <row r="43" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f>_xlfn.CONCAT("STATE_",B43)</f>
+        <f t="shared" si="4"/>
         <v>STATE_FAL</v>
       </c>
       <c r="B43" t="s">
@@ -4189,7 +4192,7 @@
     </row>
     <row r="44" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f>_xlfn.CONCAT("STATE_",B44)</f>
+        <f t="shared" si="4"/>
         <v>STATE_FALS</v>
       </c>
       <c r="B44" t="s">
@@ -4255,7 +4258,7 @@
     </row>
     <row r="45" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f>_xlfn.CONCAT("STATE_",B45)</f>
+        <f t="shared" si="4"/>
         <v xml:space="preserve">STATE_FALSE </v>
       </c>
       <c r="B45" t="s">
@@ -4318,7 +4321,7 @@
     </row>
     <row r="46" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f>_xlfn.CONCAT("STATE_",B46)</f>
+        <f t="shared" si="4"/>
         <v>STATE_TR</v>
       </c>
       <c r="B46" t="s">
@@ -4384,7 +4387,7 @@
     </row>
     <row r="47" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f>_xlfn.CONCAT("STATE_",B47)</f>
+        <f t="shared" si="4"/>
         <v>STATE_TRU</v>
       </c>
       <c r="B47" t="s">
@@ -4450,7 +4453,7 @@
     </row>
     <row r="48" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
-        <f>_xlfn.CONCAT("STATE_",B48)</f>
+        <f t="shared" si="4"/>
         <v>STATE_TRUE</v>
       </c>
       <c r="B48" t="b">
@@ -4513,7 +4516,7 @@
     </row>
     <row r="49" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
-        <f>_xlfn.CONCAT("STATE_",B49)</f>
+        <f t="shared" si="4"/>
         <v>STATE_N</v>
       </c>
       <c r="B49" t="s">
@@ -4579,7 +4582,7 @@
     </row>
     <row r="50" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
-        <f>_xlfn.CONCAT("STATE_",B50)</f>
+        <f t="shared" si="4"/>
         <v>STATE_NU</v>
       </c>
       <c r="B50" t="s">
@@ -4645,7 +4648,7 @@
     </row>
     <row r="51" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
-        <f>_xlfn.CONCAT("STATE_",B51)</f>
+        <f t="shared" si="4"/>
         <v>STATE_NUL</v>
       </c>
       <c r="B51" t="s">
@@ -4711,7 +4714,7 @@
     </row>
     <row r="52" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
-        <f>_xlfn.CONCAT("STATE_",B52)</f>
+        <f t="shared" si="4"/>
         <v>STATE_NULL</v>
       </c>
       <c r="B52" t="s">
@@ -4774,7 +4777,7 @@
     </row>
     <row r="53" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
-        <f>_xlfn.CONCAT("STATE_",B53)</f>
+        <f t="shared" si="4"/>
         <v>STATE_LPAR</v>
       </c>
       <c r="B53" t="s">
@@ -4915,7 +4918,7 @@
     </row>
     <row r="54" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
-        <f>_xlfn.CONCAT("STATE_",B54)</f>
+        <f t="shared" si="4"/>
         <v>STATE_RPAR</v>
       </c>
       <c r="B54" t="s">
@@ -5056,7 +5059,7 @@
     </row>
     <row r="55" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
-        <f>_xlfn.CONCAT("STATE_",B55)</f>
+        <f t="shared" si="4"/>
         <v>STATE_SEMIC</v>
       </c>
       <c r="B55" t="s">
@@ -5197,7 +5200,7 @@
     </row>
     <row r="56" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
-        <f>_xlfn.CONCAT("STATE_",B56)</f>
+        <f t="shared" si="4"/>
         <v>STATE_COMMA</v>
       </c>
       <c r="B56" t="s">
@@ -5338,7 +5341,7 @@
     </row>
     <row r="57" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
-        <f>_xlfn.CONCAT("STATE_",B57)</f>
+        <f t="shared" si="4"/>
         <v>STATE_COLON</v>
       </c>
       <c r="B57" t="s">
@@ -5479,7 +5482,7 @@
     </row>
     <row r="58" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
-        <f>_xlfn.CONCAT("STATE_",B58)</f>
+        <f t="shared" si="4"/>
         <v>STATE_COLONEQUALS</v>
       </c>
       <c r="B58" t="s">
@@ -5617,7 +5620,7 @@
     </row>
     <row r="59" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
-        <f>_xlfn.CONCAT("STATE_",B59)</f>
+        <f t="shared" si="4"/>
         <v>STATE_PLUS</v>
       </c>
       <c r="B59" t="s">
@@ -5755,7 +5758,7 @@
     </row>
     <row r="60" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
-        <f>_xlfn.CONCAT("STATE_",B60)</f>
+        <f t="shared" si="4"/>
         <v>STATE_MINUS</v>
       </c>
       <c r="B60" t="s">
@@ -5764,6 +5767,9 @@
       <c r="C60" t="s">
         <v>175</v>
       </c>
+      <c r="D60" t="s">
+        <v>175</v>
+      </c>
       <c r="E60" t="s">
         <v>175</v>
       </c>
@@ -5879,7 +5885,7 @@
         <v>175</v>
       </c>
       <c r="AQ60" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
       <c r="AR60" t="s">
         <v>175</v>
@@ -5893,7 +5899,7 @@
     </row>
     <row r="61" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
-        <f>_xlfn.CONCAT("STATE_",B61)</f>
+        <f t="shared" si="4"/>
         <v>STATE_MULTIPLY</v>
       </c>
       <c r="B61" t="s">
@@ -6031,7 +6037,7 @@
     </row>
     <row r="62" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
-        <f>_xlfn.CONCAT("STATE_",B62)</f>
+        <f t="shared" si="4"/>
         <v>STATE_DIV</v>
       </c>
       <c r="B62" t="s">
@@ -6169,7 +6175,7 @@
     </row>
     <row r="63" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
-        <f>_xlfn.CONCAT("STATE_",B63)</f>
+        <f t="shared" si="4"/>
         <v>STATE_NOT</v>
       </c>
       <c r="B63" t="s">
@@ -6307,7 +6313,7 @@
     </row>
     <row r="64" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
-        <f>_xlfn.CONCAT("STATE_",B64)</f>
+        <f t="shared" si="4"/>
         <v>STATE_LESS</v>
       </c>
       <c r="B64" t="s">
@@ -6445,7 +6451,7 @@
     </row>
     <row r="65" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
-        <f>_xlfn.CONCAT("STATE_",B65)</f>
+        <f t="shared" si="4"/>
         <v>STATE_LESSEQ</v>
       </c>
       <c r="B65" t="s">
@@ -6583,7 +6589,7 @@
     </row>
     <row r="66" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
-        <f>_xlfn.CONCAT("STATE_",B66)</f>
+        <f t="shared" si="4"/>
         <v>STATE_GREAT</v>
       </c>
       <c r="B66" t="s">
@@ -6721,7 +6727,7 @@
     </row>
     <row r="67" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
-        <f>_xlfn.CONCAT("STATE_",B67)</f>
+        <f t="shared" si="4"/>
         <v>STATE_GREATEQ</v>
       </c>
       <c r="B67" t="s">
@@ -6859,7 +6865,7 @@
     </row>
     <row r="68" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
-        <f>_xlfn.CONCAT("STATE_",B68)</f>
+        <f t="shared" si="4"/>
         <v>STATE_EQ</v>
       </c>
       <c r="B68" t="s">
@@ -6997,7 +7003,7 @@
     </row>
     <row r="69" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
-        <f>_xlfn.CONCAT("STATE_",B69)</f>
+        <f t="shared" ref="A69:A100" si="5">_xlfn.CONCAT("STATE_",B69)</f>
         <v>STATE_NOTEQ</v>
       </c>
       <c r="B69" t="s">
@@ -7135,7 +7141,7 @@
     </row>
     <row r="70" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
-        <f>_xlfn.CONCAT("STATE_",B70)</f>
+        <f t="shared" si="5"/>
         <v>STATE_INT</v>
       </c>
       <c r="B70" t="s">
@@ -7273,7 +7279,7 @@
     </row>
     <row r="71" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
-        <f>_xlfn.CONCAT("STATE_",B71)</f>
+        <f t="shared" si="5"/>
         <v>STATE_EOF</v>
       </c>
       <c r="B71" t="s">
@@ -7411,7 +7417,7 @@
     </row>
     <row r="72" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
-        <f>_xlfn.CONCAT("STATE_",B72)</f>
+        <f t="shared" si="5"/>
         <v>STATE_WR</v>
       </c>
       <c r="B72" t="s">
@@ -7477,7 +7483,7 @@
     </row>
     <row r="73" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
-        <f>_xlfn.CONCAT("STATE_",B73)</f>
+        <f t="shared" si="5"/>
         <v>STATE_WRI</v>
       </c>
       <c r="B73" t="s">
@@ -7543,7 +7549,7 @@
     </row>
     <row r="74" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
-        <f>_xlfn.CONCAT("STATE_",B74)</f>
+        <f t="shared" si="5"/>
         <v>STATE_WRIT</v>
       </c>
       <c r="B74" t="s">
@@ -7609,7 +7615,7 @@
     </row>
     <row r="75" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
-        <f>_xlfn.CONCAT("STATE_",B75)</f>
+        <f t="shared" si="5"/>
         <v>STATE_WRITE</v>
       </c>
       <c r="B75" t="s">
@@ -17720,7 +17726,7 @@
       </c>
       <c r="C58" t="str">
         <f>IF(Base!D60="", "STATE_ID, ID, 1", Base!D60)</f>
-        <v>STATE_ID, ID, 1</v>
+        <v>STATE_MINUS, MINUSOP, 0</v>
       </c>
       <c r="D58" t="str">
         <f>IF(Base!E60="", "STATE_ID, ID, 1", Base!E60)</f>
@@ -17876,7 +17882,7 @@
       </c>
       <c r="AP58" t="str">
         <f>IF(Base!AQ60="", "STATE_ID, ID, 1", Base!AQ60)</f>
-        <v>STATE_MINUS, MINUSOP, 0</v>
+        <v>STATE_MINUS, INTLITERAL, 1</v>
       </c>
       <c r="AQ58" t="str">
         <f>IF(Base!AR60="", "STATE_ID, ID, 1", Base!AR60)</f>
@@ -30660,7 +30666,7 @@
       </c>
       <c r="C58" t="str">
         <f>_xlfn.CONCAT("{",Filled!C58,"}")</f>
-        <v>{STATE_ID, ID, 1}</v>
+        <v>{STATE_MINUS, MINUSOP, 0}</v>
       </c>
       <c r="D58" t="str">
         <f>_xlfn.CONCAT("{",Filled!D58,"}")</f>
@@ -30816,7 +30822,7 @@
       </c>
       <c r="AP58" t="str">
         <f>_xlfn.CONCAT("{",Filled!AP58,"}")</f>
-        <v>{STATE_MINUS, MINUSOP, 0}</v>
+        <v>{STATE_MINUS, INTLITERAL, 1}</v>
       </c>
       <c r="AQ58" t="str">
         <f>_xlfn.CONCAT("{",Filled!AQ58,"}")</f>
@@ -34136,7 +34142,7 @@
       </c>
       <c r="B57" t="str">
         <f>_xlfn.CONCAT("{", _xlfn.TEXTJOIN(",",FALSE,'Array-Fied'!B58:AS58), "},")</f>
-        <v>{{STATE_MINUS, MINUSOP, 0},{STATE_ID, ID, 1},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0}},</v>
+        <v>{{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, INTLITERAL, 1},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0}},</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
final touchups on scanner
</commit_message>
<xml_diff>
--- a/docs/fullDFA.xlsx
+++ b/docs/fullDFA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karlm\Desktop\activegits\Compiler\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karl\Desktop\ghpull\Compiler-fork\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A281EB2-190F-42E9-97AF-FCFB123BECCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25C8B08-D3BB-42BF-8E2D-B48C2737661D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="390" windowWidth="19455" windowHeight="15075" xr2:uid="{793E41E3-A8D2-4B81-8F44-A7735E5B5AB8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{793E41E3-A8D2-4B81-8F44-A7735E5B5AB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="209">
   <si>
     <t>B</t>
   </si>
@@ -667,9 +667,6 @@
   <si>
     <t>STATE_FALSE, FALSEOP, 1</t>
   </si>
-  <si>
-    <t>STATE_MINUS, INTLITERAL, 1</t>
-  </si>
 </sst>
 </file>
 
@@ -1023,10 +1020,10 @@
   <dimension ref="A1:AX80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC14" sqref="AC14"/>
+      <selection pane="bottomRight" activeCell="AQ73" sqref="AQ73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5885,7 +5882,7 @@
         <v>175</v>
       </c>
       <c r="AQ60" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
       <c r="AR60" t="s">
         <v>175</v>
@@ -7003,7 +7000,7 @@
     </row>
     <row r="69" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
-        <f t="shared" ref="A69:A100" si="5">_xlfn.CONCAT("STATE_",B69)</f>
+        <f t="shared" ref="A69:A75" si="5">_xlfn.CONCAT("STATE_",B69)</f>
         <v>STATE_NOTEQ</v>
       </c>
       <c r="B69" t="s">
@@ -7148,79 +7145,82 @@
         <v>163</v>
       </c>
       <c r="C70" t="s">
-        <v>184</v>
+        <v>170</v>
+      </c>
+      <c r="D70" t="s">
+        <v>170</v>
       </c>
       <c r="E70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="F70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="G70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="H70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="I70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="J70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="K70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="L70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="M70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="N70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="O70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="P70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="Q70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="R70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="S70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="T70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="U70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="V70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="W70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="X70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="Y70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="Z70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="AA70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="AB70" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="AC70" t="s">
         <v>184</v>
@@ -7241,28 +7241,28 @@
         <v>184</v>
       </c>
       <c r="AI70" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="AJ70" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="AK70" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="AL70" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="AM70" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="AN70" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="AO70" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="AP70" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="AQ70" t="s">
         <v>144</v>
@@ -17882,7 +17882,7 @@
       </c>
       <c r="AP58" t="str">
         <f>IF(Base!AQ60="", "STATE_ID, ID, 1", Base!AQ60)</f>
-        <v>STATE_MINUS, INTLITERAL, 1</v>
+        <v>STATE_MINUS, MINUSOP, 0</v>
       </c>
       <c r="AQ58" t="str">
         <f>IF(Base!AR60="", "STATE_ID, ID, 1", Base!AR60)</f>
@@ -19542,107 +19542,107 @@
       </c>
       <c r="B68" t="str">
         <f>IF(Base!C70="", "STATE_ID, ID, 1", Base!C70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="C68" t="str">
         <f>IF(Base!D70="", "STATE_ID, ID, 1", Base!D70)</f>
-        <v>STATE_ID, ID, 1</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="D68" t="str">
         <f>IF(Base!E70="", "STATE_ID, ID, 1", Base!E70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="E68" t="str">
         <f>IF(Base!F70="", "STATE_ID, ID, 1", Base!F70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="F68" t="str">
         <f>IF(Base!G70="", "STATE_ID, ID, 1", Base!G70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="G68" t="str">
         <f>IF(Base!H70="", "STATE_ID, ID, 1", Base!H70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="H68" t="str">
         <f>IF(Base!I70="", "STATE_ID, ID, 1", Base!I70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="I68" t="str">
         <f>IF(Base!J70="", "STATE_ID, ID, 1", Base!J70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="J68" t="str">
         <f>IF(Base!K70="", "STATE_ID, ID, 1", Base!K70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="K68" t="str">
         <f>IF(Base!L70="", "STATE_ID, ID, 1", Base!L70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="L68" t="str">
         <f>IF(Base!M70="", "STATE_ID, ID, 1", Base!M70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="M68" t="str">
         <f>IF(Base!N70="", "STATE_ID, ID, 1", Base!N70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="N68" t="str">
         <f>IF(Base!O70="", "STATE_ID, ID, 1", Base!O70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="O68" t="str">
         <f>IF(Base!P70="", "STATE_ID, ID, 1", Base!P70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="P68" t="str">
         <f>IF(Base!Q70="", "STATE_ID, ID, 1", Base!Q70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="Q68" t="str">
         <f>IF(Base!R70="", "STATE_ID, ID, 1", Base!R70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="R68" t="str">
         <f>IF(Base!S70="", "STATE_ID, ID, 1", Base!S70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="S68" t="str">
         <f>IF(Base!T70="", "STATE_ID, ID, 1", Base!T70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="T68" t="str">
         <f>IF(Base!U70="", "STATE_ID, ID, 1", Base!U70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="U68" t="str">
         <f>IF(Base!V70="", "STATE_ID, ID, 1", Base!V70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="V68" t="str">
         <f>IF(Base!W70="", "STATE_ID, ID, 1", Base!W70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="W68" t="str">
         <f>IF(Base!X70="", "STATE_ID, ID, 1", Base!X70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="X68" t="str">
         <f>IF(Base!Y70="", "STATE_ID, ID, 1", Base!Y70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="Y68" t="str">
         <f>IF(Base!Z70="", "STATE_ID, ID, 1", Base!Z70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="Z68" t="str">
         <f>IF(Base!AA70="", "STATE_ID, ID, 1", Base!AA70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="AA68" t="str">
         <f>IF(Base!AB70="", "STATE_ID, ID, 1", Base!AB70)</f>
-        <v>STATE_INT, INTLITERAL, 0</v>
+        <v>STATE_ERROR, ERROR, 1</v>
       </c>
       <c r="AB68" t="str">
         <f>IF(Base!AC70="", "STATE_ID, ID, 1", Base!AC70)</f>
@@ -19670,35 +19670,35 @@
       </c>
       <c r="AH68" t="str">
         <f>IF(Base!AI70="", "STATE_ID, ID, 1", Base!AI70)</f>
-        <v>STATE_INT, INTLITERAL, 1</v>
+        <v>STATE_INT, INTLITERAL, 0</v>
       </c>
       <c r="AI68" t="str">
         <f>IF(Base!AJ70="", "STATE_ID, ID, 1", Base!AJ70)</f>
-        <v>STATE_INT, INTLITERAL, 1</v>
+        <v>STATE_INT, INTLITERAL, 0</v>
       </c>
       <c r="AJ68" t="str">
         <f>IF(Base!AK70="", "STATE_ID, ID, 1", Base!AK70)</f>
-        <v>STATE_INT, INTLITERAL, 1</v>
+        <v>STATE_INT, INTLITERAL, 0</v>
       </c>
       <c r="AK68" t="str">
         <f>IF(Base!AL70="", "STATE_ID, ID, 1", Base!AL70)</f>
-        <v>STATE_INT, INTLITERAL, 1</v>
+        <v>STATE_INT, INTLITERAL, 0</v>
       </c>
       <c r="AL68" t="str">
         <f>IF(Base!AM70="", "STATE_ID, ID, 1", Base!AM70)</f>
-        <v>STATE_INT, INTLITERAL, 1</v>
+        <v>STATE_INT, INTLITERAL, 0</v>
       </c>
       <c r="AM68" t="str">
         <f>IF(Base!AN70="", "STATE_ID, ID, 1", Base!AN70)</f>
-        <v>STATE_INT, INTLITERAL, 1</v>
+        <v>STATE_INT, INTLITERAL, 0</v>
       </c>
       <c r="AN68" t="str">
         <f>IF(Base!AO70="", "STATE_ID, ID, 1", Base!AO70)</f>
-        <v>STATE_INT, INTLITERAL, 1</v>
+        <v>STATE_INT, INTLITERAL, 0</v>
       </c>
       <c r="AO68" t="str">
         <f>IF(Base!AP70="", "STATE_ID, ID, 1", Base!AP70)</f>
-        <v>STATE_INT, INTLITERAL, 1</v>
+        <v>STATE_INT, INTLITERAL, 0</v>
       </c>
       <c r="AP68" t="str">
         <f>IF(Base!AQ70="", "STATE_ID, ID, 1", Base!AQ70)</f>
@@ -30822,7 +30822,7 @@
       </c>
       <c r="AP58" t="str">
         <f>_xlfn.CONCAT("{",Filled!AP58,"}")</f>
-        <v>{STATE_MINUS, INTLITERAL, 1}</v>
+        <v>{STATE_MINUS, MINUSOP, 0}</v>
       </c>
       <c r="AQ58" t="str">
         <f>_xlfn.CONCAT("{",Filled!AQ58,"}")</f>
@@ -32482,107 +32482,107 @@
       </c>
       <c r="B68" t="str">
         <f>_xlfn.CONCAT("{",Filled!B68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="C68" t="str">
         <f>_xlfn.CONCAT("{",Filled!C68,"}")</f>
-        <v>{STATE_ID, ID, 1}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="D68" t="str">
         <f>_xlfn.CONCAT("{",Filled!D68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="E68" t="str">
         <f>_xlfn.CONCAT("{",Filled!E68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="F68" t="str">
         <f>_xlfn.CONCAT("{",Filled!F68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="G68" t="str">
         <f>_xlfn.CONCAT("{",Filled!G68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="H68" t="str">
         <f>_xlfn.CONCAT("{",Filled!H68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="I68" t="str">
         <f>_xlfn.CONCAT("{",Filled!I68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="J68" t="str">
         <f>_xlfn.CONCAT("{",Filled!J68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="K68" t="str">
         <f>_xlfn.CONCAT("{",Filled!K68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="L68" t="str">
         <f>_xlfn.CONCAT("{",Filled!L68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="M68" t="str">
         <f>_xlfn.CONCAT("{",Filled!M68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="N68" t="str">
         <f>_xlfn.CONCAT("{",Filled!N68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="O68" t="str">
         <f>_xlfn.CONCAT("{",Filled!O68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="P68" t="str">
         <f>_xlfn.CONCAT("{",Filled!P68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="Q68" t="str">
         <f>_xlfn.CONCAT("{",Filled!Q68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="R68" t="str">
         <f>_xlfn.CONCAT("{",Filled!R68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="S68" t="str">
         <f>_xlfn.CONCAT("{",Filled!S68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="T68" t="str">
         <f>_xlfn.CONCAT("{",Filled!T68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="U68" t="str">
         <f>_xlfn.CONCAT("{",Filled!U68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="V68" t="str">
         <f>_xlfn.CONCAT("{",Filled!V68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="W68" t="str">
         <f>_xlfn.CONCAT("{",Filled!W68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="X68" t="str">
         <f>_xlfn.CONCAT("{",Filled!X68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="Y68" t="str">
         <f>_xlfn.CONCAT("{",Filled!Y68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="Z68" t="str">
         <f>_xlfn.CONCAT("{",Filled!Z68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="AA68" t="str">
         <f>_xlfn.CONCAT("{",Filled!AA68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 0}</v>
+        <v>{STATE_ERROR, ERROR, 1}</v>
       </c>
       <c r="AB68" t="str">
         <f>_xlfn.CONCAT("{",Filled!AB68,"}")</f>
@@ -32610,35 +32610,35 @@
       </c>
       <c r="AH68" t="str">
         <f>_xlfn.CONCAT("{",Filled!AH68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 1}</v>
+        <v>{STATE_INT, INTLITERAL, 0}</v>
       </c>
       <c r="AI68" t="str">
         <f>_xlfn.CONCAT("{",Filled!AI68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 1}</v>
+        <v>{STATE_INT, INTLITERAL, 0}</v>
       </c>
       <c r="AJ68" t="str">
         <f>_xlfn.CONCAT("{",Filled!AJ68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 1}</v>
+        <v>{STATE_INT, INTLITERAL, 0}</v>
       </c>
       <c r="AK68" t="str">
         <f>_xlfn.CONCAT("{",Filled!AK68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 1}</v>
+        <v>{STATE_INT, INTLITERAL, 0}</v>
       </c>
       <c r="AL68" t="str">
         <f>_xlfn.CONCAT("{",Filled!AL68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 1}</v>
+        <v>{STATE_INT, INTLITERAL, 0}</v>
       </c>
       <c r="AM68" t="str">
         <f>_xlfn.CONCAT("{",Filled!AM68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 1}</v>
+        <v>{STATE_INT, INTLITERAL, 0}</v>
       </c>
       <c r="AN68" t="str">
         <f>_xlfn.CONCAT("{",Filled!AN68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 1}</v>
+        <v>{STATE_INT, INTLITERAL, 0}</v>
       </c>
       <c r="AO68" t="str">
         <f>_xlfn.CONCAT("{",Filled!AO68,"}")</f>
-        <v>{STATE_INT, INTLITERAL, 1}</v>
+        <v>{STATE_INT, INTLITERAL, 0}</v>
       </c>
       <c r="AP68" t="str">
         <f>_xlfn.CONCAT("{",Filled!AP68,"}")</f>
@@ -33576,8 +33576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{366C0019-85C9-405F-ADC4-86E93D24BFB9}">
   <dimension ref="A2:CO72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34142,7 +34142,7 @@
       </c>
       <c r="B57" t="str">
         <f>_xlfn.CONCAT("{", _xlfn.TEXTJOIN(",",FALSE,'Array-Fied'!B58:AS58), "},")</f>
-        <v>{{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, INTLITERAL, 1},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0}},</v>
+        <v>{{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0},{STATE_MINUS, MINUSOP, 0}},</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -34242,7 +34242,7 @@
       </c>
       <c r="B67" t="str">
         <f>_xlfn.CONCAT("{", _xlfn.TEXTJOIN(",",FALSE,'Array-Fied'!B68:AS68), "},")</f>
-        <v>{{STATE_INT, INTLITERAL, 0},{STATE_ID, ID, 1},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 1},{STATE_INT, INTLITERAL, 1},{STATE_INT, INTLITERAL, 1},{STATE_INT, INTLITERAL, 1},{STATE_INT, INTLITERAL, 1},{STATE_INT, INTLITERAL, 1},{STATE_INT, INTLITERAL, 1},{STATE_INT, INTLITERAL, 1},{STATE_INT, INTLITERAL, 1},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0}},</v>
+        <v>{{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_ERROR, ERROR, 1},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 1},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0},{STATE_INT, INTLITERAL, 0}},</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>